<commit_message>
1. Implement Equipment management
</commit_message>
<xml_diff>
--- a/report_template/calibration_daily.xlsx
+++ b/report_template/calibration_daily.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>校正日報表</t>
   </si>
@@ -88,6 +88,10 @@
   <si>
     <t>全幅內控_x000D_
 偏移率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>標示說明:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -186,7 +190,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -203,19 +207,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -229,11 +239,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,74 +549,76 @@
   <dimension ref="A1:M200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="14" customWidth="1"/>
-    <col min="2" max="9" width="10.625" style="15" customWidth="1"/>
-    <col min="10" max="11" width="11.625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="10.625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="7" customWidth="1"/>
+    <col min="2" max="9" width="10.625" style="8" customWidth="1"/>
+    <col min="10" max="11" width="11.625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="10.625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="10.625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="13"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="7" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -664,7 +673,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="9"/>
+      <c r="L5" s="16"/>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -679,7 +688,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="9"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -694,7 +703,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="9"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -709,7 +718,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="9"/>
+      <c r="L8" s="16"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -724,7 +733,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="9"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -739,7 +748,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="9"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -754,7 +763,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="9"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -769,7 +778,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="9"/>
+      <c r="L12" s="16"/>
       <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -784,7 +793,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="9"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -799,7 +808,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -814,7 +823,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="9"/>
+      <c r="L15" s="16"/>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -829,7 +838,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="9"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -844,7 +853,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="9"/>
+      <c r="L17" s="16"/>
       <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -859,7 +868,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="9"/>
+      <c r="L18" s="16"/>
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -874,7 +883,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="9"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -889,7 +898,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="9"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -904,7 +913,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="9"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -919,7 +928,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="9"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -934,7 +943,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="9"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -949,7 +958,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="9"/>
+      <c r="L24" s="16"/>
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -964,7 +973,7 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="9"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -979,7 +988,7 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="9"/>
+      <c r="L26" s="16"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -994,7 +1003,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="9"/>
+      <c r="L27" s="16"/>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1009,7 +1018,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="9"/>
+      <c r="L28" s="16"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1024,7 +1033,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="9"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1039,7 +1048,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="9"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1054,7 +1063,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="9"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1069,7 +1078,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="9"/>
+      <c r="L32" s="16"/>
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1084,7 +1093,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="9"/>
+      <c r="L33" s="16"/>
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -1099,7 +1108,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="9"/>
+      <c r="L34" s="16"/>
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1114,7 +1123,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="9"/>
+      <c r="L35" s="16"/>
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -1129,7 +1138,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="9"/>
+      <c r="L36" s="16"/>
       <c r="M36" s="3"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -1144,7 +1153,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="9"/>
+      <c r="L37" s="16"/>
       <c r="M37" s="3"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -1159,7 +1168,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="9"/>
+      <c r="L38" s="16"/>
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -1174,7 +1183,7 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="9"/>
+      <c r="L39" s="16"/>
       <c r="M39" s="3"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -1189,7 +1198,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="9"/>
+      <c r="L40" s="16"/>
       <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -1204,7 +1213,7 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="9"/>
+      <c r="L41" s="16"/>
       <c r="M41" s="3"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -1219,7 +1228,7 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
-      <c r="L42" s="9"/>
+      <c r="L42" s="16"/>
       <c r="M42" s="3"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -1234,7 +1243,7 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="9"/>
+      <c r="L43" s="16"/>
       <c r="M43" s="3"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -1249,7 +1258,7 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
-      <c r="L44" s="9"/>
+      <c r="L44" s="16"/>
       <c r="M44" s="3"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -1264,7 +1273,7 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-      <c r="L45" s="9"/>
+      <c r="L45" s="16"/>
       <c r="M45" s="3"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -1279,7 +1288,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="L46" s="9"/>
+      <c r="L46" s="16"/>
       <c r="M46" s="3"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -1294,7 +1303,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
-      <c r="L47" s="9"/>
+      <c r="L47" s="16"/>
       <c r="M47" s="3"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -1309,7 +1318,7 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
-      <c r="L48" s="9"/>
+      <c r="L48" s="16"/>
       <c r="M48" s="3"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -1324,7 +1333,7 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
-      <c r="L49" s="9"/>
+      <c r="L49" s="16"/>
       <c r="M49" s="3"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -1339,7 +1348,7 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
-      <c r="L50" s="9"/>
+      <c r="L50" s="16"/>
       <c r="M50" s="3"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -1354,7 +1363,7 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
-      <c r="L51" s="9"/>
+      <c r="L51" s="16"/>
       <c r="M51" s="3"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -1369,7 +1378,7 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="9"/>
+      <c r="L52" s="16"/>
       <c r="M52" s="3"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -1384,7 +1393,7 @@
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
-      <c r="L53" s="9"/>
+      <c r="L53" s="16"/>
       <c r="M53" s="3"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -1399,7 +1408,7 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
-      <c r="L54" s="9"/>
+      <c r="L54" s="16"/>
       <c r="M54" s="3"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -1414,7 +1423,7 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
-      <c r="L55" s="9"/>
+      <c r="L55" s="16"/>
       <c r="M55" s="3"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -1429,7 +1438,7 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
-      <c r="L56" s="9"/>
+      <c r="L56" s="16"/>
       <c r="M56" s="3"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -1444,7 +1453,7 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="9"/>
+      <c r="L57" s="16"/>
       <c r="M57" s="3"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -1459,7 +1468,7 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="9"/>
+      <c r="L58" s="16"/>
       <c r="M58" s="3"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -1474,7 +1483,7 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
-      <c r="L59" s="9"/>
+      <c r="L59" s="16"/>
       <c r="M59" s="3"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -1489,7 +1498,7 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="9"/>
+      <c r="L60" s="16"/>
       <c r="M60" s="3"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -1504,7 +1513,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="9"/>
+      <c r="L61" s="16"/>
       <c r="M61" s="3"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -1519,7 +1528,7 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
-      <c r="L62" s="9"/>
+      <c r="L62" s="16"/>
       <c r="M62" s="3"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -1534,7 +1543,7 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
-      <c r="L63" s="9"/>
+      <c r="L63" s="16"/>
       <c r="M63" s="3"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -1549,7 +1558,7 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
-      <c r="L64" s="9"/>
+      <c r="L64" s="16"/>
       <c r="M64" s="3"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -1564,7 +1573,7 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="9"/>
+      <c r="L65" s="16"/>
       <c r="M65" s="3"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -1579,7 +1588,7 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
-      <c r="L66" s="9"/>
+      <c r="L66" s="16"/>
       <c r="M66" s="3"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -1594,7 +1603,7 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="9"/>
+      <c r="L67" s="16"/>
       <c r="M67" s="3"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -1609,7 +1618,7 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
-      <c r="L68" s="9"/>
+      <c r="L68" s="16"/>
       <c r="M68" s="3"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -1624,7 +1633,7 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
-      <c r="L69" s="9"/>
+      <c r="L69" s="16"/>
       <c r="M69" s="3"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -1639,7 +1648,7 @@
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
-      <c r="L70" s="9"/>
+      <c r="L70" s="16"/>
       <c r="M70" s="3"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -1654,7 +1663,7 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
-      <c r="L71" s="9"/>
+      <c r="L71" s="16"/>
       <c r="M71" s="3"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -1669,7 +1678,7 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
-      <c r="L72" s="9"/>
+      <c r="L72" s="16"/>
       <c r="M72" s="3"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -1684,7 +1693,7 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
-      <c r="L73" s="9"/>
+      <c r="L73" s="16"/>
       <c r="M73" s="3"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -1699,7 +1708,7 @@
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
-      <c r="L74" s="9"/>
+      <c r="L74" s="16"/>
       <c r="M74" s="3"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -1714,7 +1723,7 @@
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
-      <c r="L75" s="9"/>
+      <c r="L75" s="16"/>
       <c r="M75" s="3"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -1729,7 +1738,7 @@
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
-      <c r="L76" s="9"/>
+      <c r="L76" s="16"/>
       <c r="M76" s="3"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -1744,7 +1753,7 @@
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
-      <c r="L77" s="9"/>
+      <c r="L77" s="16"/>
       <c r="M77" s="3"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -1759,7 +1768,7 @@
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
-      <c r="L78" s="9"/>
+      <c r="L78" s="16"/>
       <c r="M78" s="3"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -1774,7 +1783,7 @@
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
-      <c r="L79" s="9"/>
+      <c r="L79" s="16"/>
       <c r="M79" s="3"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -1789,7 +1798,7 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
-      <c r="L80" s="9"/>
+      <c r="L80" s="16"/>
       <c r="M80" s="3"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -1804,7 +1813,7 @@
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
-      <c r="L81" s="9"/>
+      <c r="L81" s="16"/>
       <c r="M81" s="3"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -1819,7 +1828,7 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
-      <c r="L82" s="9"/>
+      <c r="L82" s="16"/>
       <c r="M82" s="3"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -1834,7 +1843,7 @@
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
-      <c r="L83" s="9"/>
+      <c r="L83" s="16"/>
       <c r="M83" s="3"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -1849,7 +1858,7 @@
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
-      <c r="L84" s="9"/>
+      <c r="L84" s="16"/>
       <c r="M84" s="3"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -1864,7 +1873,7 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
-      <c r="L85" s="9"/>
+      <c r="L85" s="16"/>
       <c r="M85" s="3"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -1879,7 +1888,7 @@
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
-      <c r="L86" s="9"/>
+      <c r="L86" s="16"/>
       <c r="M86" s="3"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -1894,7 +1903,7 @@
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
-      <c r="L87" s="9"/>
+      <c r="L87" s="16"/>
       <c r="M87" s="3"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -1909,7 +1918,7 @@
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
-      <c r="L88" s="9"/>
+      <c r="L88" s="16"/>
       <c r="M88" s="3"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -1924,7 +1933,7 @@
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
-      <c r="L89" s="9"/>
+      <c r="L89" s="16"/>
       <c r="M89" s="3"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -1939,7 +1948,7 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
-      <c r="L90" s="9"/>
+      <c r="L90" s="16"/>
       <c r="M90" s="3"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -1954,7 +1963,7 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
-      <c r="L91" s="9"/>
+      <c r="L91" s="16"/>
       <c r="M91" s="3"/>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -1969,7 +1978,7 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
-      <c r="L92" s="9"/>
+      <c r="L92" s="16"/>
       <c r="M92" s="3"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -1984,7 +1993,7 @@
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
-      <c r="L93" s="9"/>
+      <c r="L93" s="16"/>
       <c r="M93" s="3"/>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
@@ -1999,7 +2008,7 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
-      <c r="L94" s="9"/>
+      <c r="L94" s="16"/>
       <c r="M94" s="3"/>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -2014,7 +2023,7 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
-      <c r="L95" s="9"/>
+      <c r="L95" s="16"/>
       <c r="M95" s="3"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
@@ -2029,7 +2038,7 @@
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
-      <c r="L96" s="9"/>
+      <c r="L96" s="16"/>
       <c r="M96" s="3"/>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -2044,7 +2053,7 @@
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
-      <c r="L97" s="9"/>
+      <c r="L97" s="16"/>
       <c r="M97" s="3"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -2059,7 +2068,7 @@
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
-      <c r="L98" s="9"/>
+      <c r="L98" s="16"/>
       <c r="M98" s="3"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
@@ -2074,7 +2083,7 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
-      <c r="L99" s="9"/>
+      <c r="L99" s="16"/>
       <c r="M99" s="3"/>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -2089,7 +2098,7 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
-      <c r="L100" s="9"/>
+      <c r="L100" s="16"/>
       <c r="M100" s="3"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
@@ -2104,7 +2113,7 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
-      <c r="L101" s="9"/>
+      <c r="L101" s="16"/>
       <c r="M101" s="3"/>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
@@ -2119,7 +2128,7 @@
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
-      <c r="L102" s="9"/>
+      <c r="L102" s="16"/>
       <c r="M102" s="3"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
@@ -2134,7 +2143,7 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
-      <c r="L103" s="9"/>
+      <c r="L103" s="16"/>
       <c r="M103" s="3"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
@@ -2149,7 +2158,7 @@
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
-      <c r="L104" s="9"/>
+      <c r="L104" s="16"/>
       <c r="M104" s="3"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
@@ -2164,7 +2173,7 @@
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
-      <c r="L105" s="9"/>
+      <c r="L105" s="6"/>
       <c r="M105" s="3"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
@@ -2179,7 +2188,7 @@
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
-      <c r="L106" s="9"/>
+      <c r="L106" s="6"/>
       <c r="M106" s="3"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
@@ -2194,7 +2203,7 @@
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
-      <c r="L107" s="9"/>
+      <c r="L107" s="6"/>
       <c r="M107" s="3"/>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
@@ -2209,7 +2218,7 @@
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
-      <c r="L108" s="9"/>
+      <c r="L108" s="6"/>
       <c r="M108" s="3"/>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
@@ -2224,7 +2233,7 @@
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
-      <c r="L109" s="9"/>
+      <c r="L109" s="6"/>
       <c r="M109" s="3"/>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
@@ -2239,7 +2248,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
-      <c r="L110" s="9"/>
+      <c r="L110" s="6"/>
       <c r="M110" s="3"/>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
@@ -2254,7 +2263,7 @@
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
-      <c r="L111" s="9"/>
+      <c r="L111" s="6"/>
       <c r="M111" s="3"/>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
@@ -2269,7 +2278,7 @@
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
-      <c r="L112" s="9"/>
+      <c r="L112" s="6"/>
       <c r="M112" s="3"/>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
@@ -2284,7 +2293,7 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
-      <c r="L113" s="9"/>
+      <c r="L113" s="6"/>
       <c r="M113" s="3"/>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
@@ -2299,7 +2308,7 @@
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
-      <c r="L114" s="9"/>
+      <c r="L114" s="6"/>
       <c r="M114" s="3"/>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
@@ -2314,7 +2323,7 @@
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
-      <c r="L115" s="9"/>
+      <c r="L115" s="6"/>
       <c r="M115" s="3"/>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
@@ -2329,7 +2338,7 @@
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
-      <c r="L116" s="9"/>
+      <c r="L116" s="6"/>
       <c r="M116" s="3"/>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
@@ -2344,7 +2353,7 @@
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
-      <c r="L117" s="9"/>
+      <c r="L117" s="6"/>
       <c r="M117" s="3"/>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
@@ -2359,7 +2368,7 @@
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
-      <c r="L118" s="9"/>
+      <c r="L118" s="6"/>
       <c r="M118" s="3"/>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
@@ -2374,7 +2383,7 @@
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
-      <c r="L119" s="9"/>
+      <c r="L119" s="6"/>
       <c r="M119" s="3"/>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
@@ -2389,7 +2398,7 @@
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
-      <c r="L120" s="9"/>
+      <c r="L120" s="6"/>
       <c r="M120" s="3"/>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
@@ -2404,7 +2413,7 @@
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
-      <c r="L121" s="9"/>
+      <c r="L121" s="6"/>
       <c r="M121" s="3"/>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
@@ -2419,7 +2428,7 @@
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
-      <c r="L122" s="9"/>
+      <c r="L122" s="6"/>
       <c r="M122" s="3"/>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
@@ -2434,7 +2443,7 @@
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
-      <c r="L123" s="9"/>
+      <c r="L123" s="6"/>
       <c r="M123" s="3"/>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
@@ -2449,7 +2458,7 @@
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
-      <c r="L124" s="9"/>
+      <c r="L124" s="6"/>
       <c r="M124" s="3"/>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
@@ -2464,7 +2473,7 @@
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
-      <c r="L125" s="9"/>
+      <c r="L125" s="6"/>
       <c r="M125" s="3"/>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
@@ -2479,7 +2488,7 @@
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
-      <c r="L126" s="9"/>
+      <c r="L126" s="6"/>
       <c r="M126" s="3"/>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
@@ -2494,7 +2503,7 @@
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
-      <c r="L127" s="9"/>
+      <c r="L127" s="6"/>
       <c r="M127" s="3"/>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
@@ -2509,7 +2518,7 @@
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
-      <c r="L128" s="9"/>
+      <c r="L128" s="6"/>
       <c r="M128" s="3"/>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
@@ -2524,7 +2533,7 @@
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
-      <c r="L129" s="9"/>
+      <c r="L129" s="6"/>
       <c r="M129" s="3"/>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
@@ -2539,7 +2548,7 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3"/>
-      <c r="L130" s="9"/>
+      <c r="L130" s="6"/>
       <c r="M130" s="3"/>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
@@ -2554,7 +2563,7 @@
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
-      <c r="L131" s="9"/>
+      <c r="L131" s="6"/>
       <c r="M131" s="3"/>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
@@ -2569,7 +2578,7 @@
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
-      <c r="L132" s="9"/>
+      <c r="L132" s="6"/>
       <c r="M132" s="3"/>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
@@ -2584,7 +2593,7 @@
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
-      <c r="L133" s="9"/>
+      <c r="L133" s="6"/>
       <c r="M133" s="3"/>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
@@ -2599,7 +2608,7 @@
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
-      <c r="L134" s="9"/>
+      <c r="L134" s="6"/>
       <c r="M134" s="3"/>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
@@ -2614,7 +2623,7 @@
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
-      <c r="L135" s="9"/>
+      <c r="L135" s="6"/>
       <c r="M135" s="3"/>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
@@ -2629,7 +2638,7 @@
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
-      <c r="L136" s="9"/>
+      <c r="L136" s="6"/>
       <c r="M136" s="3"/>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
@@ -2644,7 +2653,7 @@
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
-      <c r="L137" s="9"/>
+      <c r="L137" s="6"/>
       <c r="M137" s="3"/>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
@@ -2659,7 +2668,7 @@
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
-      <c r="L138" s="9"/>
+      <c r="L138" s="6"/>
       <c r="M138" s="3"/>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
@@ -2674,7 +2683,7 @@
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
-      <c r="L139" s="9"/>
+      <c r="L139" s="6"/>
       <c r="M139" s="3"/>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
@@ -2689,7 +2698,7 @@
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
       <c r="K140" s="3"/>
-      <c r="L140" s="9"/>
+      <c r="L140" s="6"/>
       <c r="M140" s="3"/>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
@@ -2704,7 +2713,7 @@
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
-      <c r="L141" s="9"/>
+      <c r="L141" s="6"/>
       <c r="M141" s="3"/>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
@@ -2719,7 +2728,7 @@
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
-      <c r="L142" s="9"/>
+      <c r="L142" s="6"/>
       <c r="M142" s="3"/>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
@@ -2734,7 +2743,7 @@
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
       <c r="K143" s="3"/>
-      <c r="L143" s="9"/>
+      <c r="L143" s="6"/>
       <c r="M143" s="3"/>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
@@ -2749,7 +2758,7 @@
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
-      <c r="L144" s="9"/>
+      <c r="L144" s="6"/>
       <c r="M144" s="3"/>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
@@ -2764,7 +2773,7 @@
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
-      <c r="L145" s="9"/>
+      <c r="L145" s="6"/>
       <c r="M145" s="3"/>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
@@ -2779,7 +2788,7 @@
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
-      <c r="L146" s="9"/>
+      <c r="L146" s="6"/>
       <c r="M146" s="3"/>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
@@ -2794,7 +2803,7 @@
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
-      <c r="L147" s="9"/>
+      <c r="L147" s="6"/>
       <c r="M147" s="3"/>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
@@ -2809,7 +2818,7 @@
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
-      <c r="L148" s="9"/>
+      <c r="L148" s="6"/>
       <c r="M148" s="3"/>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -2824,7 +2833,7 @@
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
       <c r="K149" s="3"/>
-      <c r="L149" s="9"/>
+      <c r="L149" s="6"/>
       <c r="M149" s="3"/>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -2839,7 +2848,7 @@
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
-      <c r="L150" s="9"/>
+      <c r="L150" s="6"/>
       <c r="M150" s="3"/>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
@@ -2854,7 +2863,7 @@
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
-      <c r="L151" s="9"/>
+      <c r="L151" s="6"/>
       <c r="M151" s="3"/>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
@@ -2869,7 +2878,7 @@
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
       <c r="K152" s="3"/>
-      <c r="L152" s="9"/>
+      <c r="L152" s="6"/>
       <c r="M152" s="3"/>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
@@ -2884,7 +2893,7 @@
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
-      <c r="L153" s="9"/>
+      <c r="L153" s="6"/>
       <c r="M153" s="3"/>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
@@ -2899,7 +2908,7 @@
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
-      <c r="L154" s="9"/>
+      <c r="L154" s="6"/>
       <c r="M154" s="3"/>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
@@ -2914,7 +2923,7 @@
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
-      <c r="L155" s="9"/>
+      <c r="L155" s="6"/>
       <c r="M155" s="3"/>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
@@ -2929,7 +2938,7 @@
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
-      <c r="L156" s="9"/>
+      <c r="L156" s="6"/>
       <c r="M156" s="3"/>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
@@ -2944,7 +2953,7 @@
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
-      <c r="L157" s="9"/>
+      <c r="L157" s="6"/>
       <c r="M157" s="3"/>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
@@ -2959,7 +2968,7 @@
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
-      <c r="L158" s="9"/>
+      <c r="L158" s="6"/>
       <c r="M158" s="3"/>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
@@ -2974,7 +2983,7 @@
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
-      <c r="L159" s="9"/>
+      <c r="L159" s="6"/>
       <c r="M159" s="3"/>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -2989,7 +2998,7 @@
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
-      <c r="L160" s="9"/>
+      <c r="L160" s="6"/>
       <c r="M160" s="3"/>
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
@@ -3004,7 +3013,7 @@
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
-      <c r="L161" s="9"/>
+      <c r="L161" s="6"/>
       <c r="M161" s="3"/>
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
@@ -3019,7 +3028,7 @@
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
       <c r="K162" s="3"/>
-      <c r="L162" s="9"/>
+      <c r="L162" s="6"/>
       <c r="M162" s="3"/>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
@@ -3034,7 +3043,7 @@
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
-      <c r="L163" s="9"/>
+      <c r="L163" s="6"/>
       <c r="M163" s="3"/>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
@@ -3049,7 +3058,7 @@
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
-      <c r="L164" s="9"/>
+      <c r="L164" s="6"/>
       <c r="M164" s="3"/>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
@@ -3064,7 +3073,7 @@
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
       <c r="K165" s="3"/>
-      <c r="L165" s="9"/>
+      <c r="L165" s="6"/>
       <c r="M165" s="3"/>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
@@ -3079,7 +3088,7 @@
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
-      <c r="L166" s="9"/>
+      <c r="L166" s="6"/>
       <c r="M166" s="3"/>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
@@ -3094,7 +3103,7 @@
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
-      <c r="L167" s="9"/>
+      <c r="L167" s="6"/>
       <c r="M167" s="3"/>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
@@ -3109,7 +3118,7 @@
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
-      <c r="L168" s="9"/>
+      <c r="L168" s="6"/>
       <c r="M168" s="3"/>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
@@ -3124,7 +3133,7 @@
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
-      <c r="L169" s="9"/>
+      <c r="L169" s="6"/>
       <c r="M169" s="3"/>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
@@ -3139,7 +3148,7 @@
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
       <c r="K170" s="3"/>
-      <c r="L170" s="9"/>
+      <c r="L170" s="6"/>
       <c r="M170" s="3"/>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
@@ -3154,7 +3163,7 @@
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
-      <c r="L171" s="9"/>
+      <c r="L171" s="6"/>
       <c r="M171" s="3"/>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
@@ -3169,7 +3178,7 @@
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
-      <c r="L172" s="9"/>
+      <c r="L172" s="6"/>
       <c r="M172" s="3"/>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
@@ -3184,7 +3193,7 @@
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
-      <c r="L173" s="9"/>
+      <c r="L173" s="6"/>
       <c r="M173" s="3"/>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
@@ -3199,7 +3208,7 @@
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
       <c r="K174" s="3"/>
-      <c r="L174" s="9"/>
+      <c r="L174" s="6"/>
       <c r="M174" s="3"/>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
@@ -3214,7 +3223,7 @@
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
-      <c r="L175" s="9"/>
+      <c r="L175" s="6"/>
       <c r="M175" s="3"/>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
@@ -3229,7 +3238,7 @@
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
       <c r="K176" s="3"/>
-      <c r="L176" s="9"/>
+      <c r="L176" s="6"/>
       <c r="M176" s="3"/>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.25">
@@ -3244,7 +3253,7 @@
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
       <c r="K177" s="3"/>
-      <c r="L177" s="9"/>
+      <c r="L177" s="6"/>
       <c r="M177" s="3"/>
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.25">
@@ -3259,7 +3268,7 @@
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
       <c r="K178" s="3"/>
-      <c r="L178" s="9"/>
+      <c r="L178" s="6"/>
       <c r="M178" s="3"/>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.25">
@@ -3274,7 +3283,7 @@
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
       <c r="K179" s="3"/>
-      <c r="L179" s="9"/>
+      <c r="L179" s="6"/>
       <c r="M179" s="3"/>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.25">
@@ -3289,7 +3298,7 @@
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
       <c r="K180" s="3"/>
-      <c r="L180" s="9"/>
+      <c r="L180" s="6"/>
       <c r="M180" s="3"/>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.25">
@@ -3304,7 +3313,7 @@
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
       <c r="K181" s="3"/>
-      <c r="L181" s="9"/>
+      <c r="L181" s="6"/>
       <c r="M181" s="3"/>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.25">
@@ -3319,7 +3328,7 @@
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
       <c r="K182" s="3"/>
-      <c r="L182" s="9"/>
+      <c r="L182" s="6"/>
       <c r="M182" s="3"/>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.25">
@@ -3334,7 +3343,7 @@
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
       <c r="K183" s="3"/>
-      <c r="L183" s="9"/>
+      <c r="L183" s="6"/>
       <c r="M183" s="3"/>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.25">
@@ -3349,7 +3358,7 @@
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
       <c r="K184" s="3"/>
-      <c r="L184" s="9"/>
+      <c r="L184" s="6"/>
       <c r="M184" s="3"/>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.25">
@@ -3364,7 +3373,7 @@
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
       <c r="K185" s="3"/>
-      <c r="L185" s="9"/>
+      <c r="L185" s="6"/>
       <c r="M185" s="3"/>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.25">
@@ -3379,7 +3388,7 @@
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
       <c r="K186" s="3"/>
-      <c r="L186" s="9"/>
+      <c r="L186" s="6"/>
       <c r="M186" s="3"/>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.25">
@@ -3394,7 +3403,7 @@
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
       <c r="K187" s="3"/>
-      <c r="L187" s="9"/>
+      <c r="L187" s="6"/>
       <c r="M187" s="3"/>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.25">
@@ -3409,7 +3418,7 @@
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
       <c r="K188" s="3"/>
-      <c r="L188" s="9"/>
+      <c r="L188" s="6"/>
       <c r="M188" s="3"/>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
@@ -3424,7 +3433,7 @@
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
       <c r="K189" s="3"/>
-      <c r="L189" s="9"/>
+      <c r="L189" s="6"/>
       <c r="M189" s="3"/>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.25">
@@ -3439,7 +3448,7 @@
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
       <c r="K190" s="3"/>
-      <c r="L190" s="9"/>
+      <c r="L190" s="6"/>
       <c r="M190" s="3"/>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.25">
@@ -3454,7 +3463,7 @@
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
       <c r="K191" s="3"/>
-      <c r="L191" s="9"/>
+      <c r="L191" s="6"/>
       <c r="M191" s="3"/>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.25">
@@ -3469,7 +3478,7 @@
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
       <c r="K192" s="3"/>
-      <c r="L192" s="9"/>
+      <c r="L192" s="6"/>
       <c r="M192" s="3"/>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.25">
@@ -3484,7 +3493,7 @@
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
       <c r="K193" s="3"/>
-      <c r="L193" s="9"/>
+      <c r="L193" s="6"/>
       <c r="M193" s="3"/>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.25">
@@ -3499,7 +3508,7 @@
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
       <c r="K194" s="3"/>
-      <c r="L194" s="9"/>
+      <c r="L194" s="6"/>
       <c r="M194" s="3"/>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.25">
@@ -3514,7 +3523,7 @@
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
       <c r="K195" s="3"/>
-      <c r="L195" s="9"/>
+      <c r="L195" s="6"/>
       <c r="M195" s="3"/>
     </row>
     <row r="196" spans="1:13" x14ac:dyDescent="0.25">
@@ -3529,7 +3538,7 @@
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
       <c r="K196" s="3"/>
-      <c r="L196" s="9"/>
+      <c r="L196" s="6"/>
       <c r="M196" s="3"/>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
@@ -3544,7 +3553,7 @@
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
       <c r="K197" s="3"/>
-      <c r="L197" s="9"/>
+      <c r="L197" s="6"/>
       <c r="M197" s="3"/>
     </row>
     <row r="198" spans="1:13" x14ac:dyDescent="0.25">
@@ -3559,7 +3568,7 @@
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
       <c r="K198" s="3"/>
-      <c r="L198" s="9"/>
+      <c r="L198" s="6"/>
       <c r="M198" s="3"/>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.25">
@@ -3574,7 +3583,7 @@
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
       <c r="K199" s="3"/>
-      <c r="L199" s="9"/>
+      <c r="L199" s="6"/>
       <c r="M199" s="3"/>
     </row>
     <row r="200" spans="1:13" x14ac:dyDescent="0.25">
@@ -3589,7 +3598,7 @@
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
       <c r="K200" s="3"/>
-      <c r="L200" s="9"/>
+      <c r="L200" s="6"/>
       <c r="M200" s="3"/>
     </row>
   </sheetData>

</xml_diff>